<commit_message>
Ajout des descriptions des instructions
</commit_message>
<xml_diff>
--- a/InstructionList.xlsx
+++ b/InstructionList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>Opcode</t>
   </si>
@@ -243,13 +243,118 @@
   </si>
   <si>
     <t>0x4XNN</t>
+  </si>
+  <si>
+    <t>Calls RCA 1802 program at address NNN. Not necessary for most ROMs.</t>
+  </si>
+  <si>
+    <t>Clears the screen.</t>
+  </si>
+  <si>
+    <t>Returns from a subroutine.</t>
+  </si>
+  <si>
+    <t>Jumps to address NNN.</t>
+  </si>
+  <si>
+    <t>Calls subroutine at NNN.</t>
+  </si>
+  <si>
+    <t>Skips the next instruction if VX equals NN.</t>
+  </si>
+  <si>
+    <t>Skips the next instruction if VX doesn't equal NN.</t>
+  </si>
+  <si>
+    <t>Skips the next instruction if VX equals VY.</t>
+  </si>
+  <si>
+    <t>Sets VX to NN.</t>
+  </si>
+  <si>
+    <t>Adds NN to VX.</t>
+  </si>
+  <si>
+    <t>Sets VX to the value of VY.</t>
+  </si>
+  <si>
+    <t>Sets VX to VX or VY.</t>
+  </si>
+  <si>
+    <t>Sets VX to VX and VY.</t>
+  </si>
+  <si>
+    <t>Sets VX to VX xor VY.</t>
+  </si>
+  <si>
+    <t>Adds VY to VX. VF is set to 1 when there's a carry, and to 0 when there isn't.</t>
+  </si>
+  <si>
+    <t>VY is subtracted from VX. VF is set to 0 when there's a borrow, and 1 when there isn't.</t>
+  </si>
+  <si>
+    <t>Shifts VX right by one. VF is set to the value of the least significant bit of VX before the shift.</t>
+  </si>
+  <si>
+    <t>Sets VX to VY minus VX. VF is set to 0 when there's a borrow, and 1 when there isn't.</t>
+  </si>
+  <si>
+    <t>Shifts VX left by one. VF is set to the value of the most significant bit of VX before the shift.</t>
+  </si>
+  <si>
+    <t>Skips the next instruction if VX doesn't equal VY.</t>
+  </si>
+  <si>
+    <t>Sets I to the address NNN.</t>
+  </si>
+  <si>
+    <t>Jumps to the address NNN plus V0.</t>
+  </si>
+  <si>
+    <t>Sets VX to the result of a bitwise and operation on a random number and NN.</t>
+  </si>
+  <si>
+    <t>Sprites stored in memory at location in index register (I), 8bits wide. Wraps around the screen. If when drawn, clears a pixel, register VF is set to 1 otherwise it is zero. All drawing is XOR drawing (i.e. it toggles the screen pixels). Sprites are drawn starting at position VX, VY. N is the number of 8bit rows that need to be drawn. If N is greater than 1, second line continues at position VX, VY+1, and so on.</t>
+  </si>
+  <si>
+    <t>Skips the next instruction if the key stored in VX is pressed.</t>
+  </si>
+  <si>
+    <t>Skips the next instruction if the key stored in VX isn't pressed.</t>
+  </si>
+  <si>
+    <t>Sets VX to the value of the delay timer.</t>
+  </si>
+  <si>
+    <t>A key press is awaited, and then stored in VX.</t>
+  </si>
+  <si>
+    <t>Sets the delay timer to VX.</t>
+  </si>
+  <si>
+    <t>Sets the sound timer to VX.</t>
+  </si>
+  <si>
+    <t>Adds VX to I.</t>
+  </si>
+  <si>
+    <t>Sets I to the location of the sprite for the character in VX. Characters 0-F (in hexadecimal) are represented by a 4x5 font.</t>
+  </si>
+  <si>
+    <t>Stores the Binary-coded decimal representation of VX, with the most significant of three digits at the address in I, the middle digit at I plus 1, and the least significant digit at I plus 2. (In other words, take the decimal representation of VX, place the hundreds digit in memory at location in I, the tens digit at location I+1, and the ones digit at location I+2.)</t>
+  </si>
+  <si>
+    <t>Stores V0 to VX in memory starting at address I.</t>
+  </si>
+  <si>
+    <t>Fills V0 to VX with values from memory starting at address I.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +366,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -286,17 +398,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -310,12 +483,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:C36" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:C36" totalsRowShown="0" dataDxfId="0">
   <autoFilter ref="A1:C36"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Opcode"/>
-    <tableColumn id="2" name="Assembleur"/>
-    <tableColumn id="3" name="Explication"/>
+    <tableColumn id="1" name="Opcode" dataDxfId="3"/>
+    <tableColumn id="2" name="Assembleur" dataDxfId="2"/>
+    <tableColumn id="3" name="Explication" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -586,14 +759,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="1" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="91.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -609,283 +781,388 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="C10" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="C11" s="3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C16" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C17" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C18" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C19" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C20" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C21" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C22" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C23" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C24" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C25" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C26" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C27" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C28" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C29" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C30" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C31" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C32" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C33" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C34" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C35" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>63</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>